<commit_message>
van dag naar per uur
</commit_message>
<xml_diff>
--- a/uurschema_voorbeeld.xlsx
+++ b/uurschema_voorbeeld.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmvpaeme/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED0B36-E1BB-B44E-BC9E-267E5EFAABBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDFF6D2-0A2D-904B-AAE1-A9CAB6F2CAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="1060" windowWidth="28040" windowHeight="16940" xr2:uid="{5349E401-A4A1-4448-B434-73B61E02F742}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>dag</t>
   </si>
@@ -45,13 +45,16 @@
     <t>uitgetikt</t>
   </si>
   <si>
-    <t>wacht</t>
-  </si>
-  <si>
-    <t>verlof</t>
-  </si>
-  <si>
-    <t>recup</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A5E442-3328-8A4F-83BD-5224EBAC2DE8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -416,9 +419,10 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,14 +435,8 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44470</v>
       </c>
@@ -448,8 +446,9 @@
       <c r="C2" s="2">
         <v>44470.875</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44471</v>
       </c>
@@ -459,8 +458,9 @@
       <c r="C3" s="2">
         <v>44471.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44472</v>
       </c>
@@ -470,64 +470,76 @@
       <c r="C4" s="2">
         <v>44473.333333333336</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>44473</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>44474</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
         <v>44474.291666666664</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>44474.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>44475</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>44475.291666666664</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <v>44475.875</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>44476</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>44477</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <v>44477</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>44511</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>44511.291666666664</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="2">
         <v>44511.75</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
+      <c r="D10" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>